<commit_message>
added Sarima Model for Telangana
</commit_message>
<xml_diff>
--- a/Telangana/Future_Predicted_TG.xlsx
+++ b/Telangana/Future_Predicted_TG.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\karti\Desktop\Arima &amp; Sarima - COVID\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My Projects\DIC Projects\COVID Trend Analysis\Arima &amp; Sarima Models - COVID Trend Analysis\SARIMA\Telangana\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39748BC3-A808-4EC7-9D92-7F3D5F1033FE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4851220-BF09-4CA2-8165-047EAAF32B62}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,11 +16,6 @@
     <sheet name="4457aed65ed8895d5e26de5cc653f91" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
-  <extLst>
-    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="CalcA1"/>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
@@ -39,79 +34,79 @@
     <t>Future_Predicted_Decreased</t>
   </si>
   <si>
-    <t>2020-06-12</t>
-  </si>
-  <si>
-    <t>2020-06-13</t>
-  </si>
-  <si>
-    <t>2020-06-14</t>
-  </si>
-  <si>
-    <t>2020-06-15</t>
-  </si>
-  <si>
-    <t>2020-06-16</t>
-  </si>
-  <si>
-    <t>2020-06-17</t>
-  </si>
-  <si>
-    <t>2020-06-18</t>
-  </si>
-  <si>
-    <t>2020-06-19</t>
-  </si>
-  <si>
-    <t>2020-06-20</t>
-  </si>
-  <si>
-    <t>2020-06-21</t>
-  </si>
-  <si>
-    <t>2020-06-22</t>
-  </si>
-  <si>
-    <t>2020-06-23</t>
-  </si>
-  <si>
-    <t>2020-06-24</t>
-  </si>
-  <si>
-    <t>2020-06-25</t>
-  </si>
-  <si>
-    <t>2020-06-26</t>
-  </si>
-  <si>
-    <t>2020-06-27</t>
-  </si>
-  <si>
-    <t>2020-06-28</t>
-  </si>
-  <si>
-    <t>2020-06-29</t>
-  </si>
-  <si>
-    <t>2020-06-30</t>
-  </si>
-  <si>
-    <t>2020-07-01</t>
-  </si>
-  <si>
-    <t>2020-07-02</t>
-  </si>
-  <si>
-    <t>2020-07-03</t>
-  </si>
-  <si>
-    <t>2020-07-04</t>
-  </si>
-  <si>
-    <t>2020-07-05</t>
-  </si>
-  <si>
-    <t>2020-07-06</t>
+    <t>2020-07-07</t>
+  </si>
+  <si>
+    <t>2020-07-08</t>
+  </si>
+  <si>
+    <t>2020-07-09</t>
+  </si>
+  <si>
+    <t>2020-07-10</t>
+  </si>
+  <si>
+    <t>2020-07-11</t>
+  </si>
+  <si>
+    <t>2020-07-12</t>
+  </si>
+  <si>
+    <t>2020-07-13</t>
+  </si>
+  <si>
+    <t>2020-07-14</t>
+  </si>
+  <si>
+    <t>2020-07-15</t>
+  </si>
+  <si>
+    <t>2020-07-16</t>
+  </si>
+  <si>
+    <t>2020-07-17</t>
+  </si>
+  <si>
+    <t>2020-07-18</t>
+  </si>
+  <si>
+    <t>2020-07-19</t>
+  </si>
+  <si>
+    <t>2020-07-20</t>
+  </si>
+  <si>
+    <t>2020-07-21</t>
+  </si>
+  <si>
+    <t>2020-07-22</t>
+  </si>
+  <si>
+    <t>2020-07-23</t>
+  </si>
+  <si>
+    <t>2020-07-24</t>
+  </si>
+  <si>
+    <t>2020-07-25</t>
+  </si>
+  <si>
+    <t>2020-07-26</t>
+  </si>
+  <si>
+    <t>2020-07-27</t>
+  </si>
+  <si>
+    <t>2020-07-28</t>
+  </si>
+  <si>
+    <t>2020-07-29</t>
+  </si>
+  <si>
+    <t>2020-07-30</t>
+  </si>
+  <si>
+    <t>2020-07-31</t>
   </si>
 </sst>
 </file>
@@ -145,7 +140,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
@@ -601,9 +597,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
@@ -613,367 +607,367 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B2">
-        <v>252.328204591196</v>
-      </c>
-      <c r="C2">
-        <v>137.35622711864201</v>
-      </c>
-      <c r="D2">
-        <v>9.9827291895561405</v>
+      <c r="B2" s="1">
+        <v>793.18435480494304</v>
+      </c>
+      <c r="C2" s="1">
+        <v>728.00136739957395</v>
+      </c>
+      <c r="D2" s="1">
+        <v>21.351463054583199</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B3">
-        <v>243.721550630422</v>
-      </c>
-      <c r="C3">
-        <v>123.890773990426</v>
-      </c>
-      <c r="D3">
-        <v>12.6283422391852</v>
+      <c r="B3" s="1">
+        <v>791.24240463880994</v>
+      </c>
+      <c r="C3" s="1">
+        <v>799.52043194362795</v>
+      </c>
+      <c r="D3" s="1">
+        <v>17.609751960960299</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B4">
-        <v>228.995013408484</v>
-      </c>
-      <c r="C4">
-        <v>142.17037364442299</v>
-      </c>
-      <c r="D4">
-        <v>8.5299087329658203</v>
+      <c r="B4" s="1">
+        <v>888.99717085417399</v>
+      </c>
+      <c r="C4" s="1">
+        <v>800.31236633065998</v>
+      </c>
+      <c r="D4" s="1">
+        <v>19.018346467165902</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B5">
-        <v>304.35792441655201</v>
-      </c>
-      <c r="C5">
-        <v>150.870059732447</v>
-      </c>
-      <c r="D5">
-        <v>9.6789838337240592</v>
+      <c r="B5" s="1">
+        <v>890.02881369800798</v>
+      </c>
+      <c r="C5" s="1">
+        <v>837.73715192645102</v>
+      </c>
+      <c r="D5" s="1">
+        <v>22.769909124500099</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B6">
-        <v>288.46985547509399</v>
-      </c>
-      <c r="C6">
-        <v>171.26901787399001</v>
-      </c>
-      <c r="D6">
-        <v>12.9648523512568</v>
+      <c r="B6" s="1">
+        <v>888.84948328613098</v>
+      </c>
+      <c r="C6" s="1">
+        <v>913.90279904756801</v>
+      </c>
+      <c r="D6" s="1">
+        <v>19.024507933104601</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B7">
-        <v>269.41366555125899</v>
-      </c>
-      <c r="C7">
-        <v>220.53477562582299</v>
-      </c>
-      <c r="D7">
-        <v>9.4042715792826694</v>
+      <c r="B7" s="1">
+        <v>990.96350278987302</v>
+      </c>
+      <c r="C7" s="1">
+        <v>915.84416738137202</v>
+      </c>
+      <c r="D7" s="1">
+        <v>20.477187527144299</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B8">
-        <v>343.97827136774401</v>
-      </c>
-      <c r="C8">
-        <v>203.31280521622801</v>
-      </c>
-      <c r="D8">
-        <v>10.410450287879</v>
+      <c r="B8" s="1">
+        <v>993.76096781642195</v>
+      </c>
+      <c r="C8" s="1">
+        <v>956.18202182351695</v>
+      </c>
+      <c r="D8" s="1">
+        <v>24.320059809677002</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B9">
-        <v>343.98624901760797</v>
-      </c>
-      <c r="C9">
-        <v>232.56786078450199</v>
-      </c>
-      <c r="D9">
-        <v>13.0925114705884</v>
+      <c r="B9" s="1">
+        <v>994.52520608766395</v>
+      </c>
+      <c r="C9" s="1">
+        <v>1036.3525391948201</v>
+      </c>
+      <c r="D9" s="1">
+        <v>20.495265665288802</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B10">
-        <v>343.06558035412502</v>
-      </c>
-      <c r="C10">
-        <v>293.846940207567</v>
-      </c>
-      <c r="D10">
-        <v>10.960464002659499</v>
+      <c r="B10" s="1">
+        <v>1100.45603216682</v>
+      </c>
+      <c r="C10" s="1">
+        <v>1040.45059001139</v>
+      </c>
+      <c r="D10" s="1">
+        <v>22.000995207489598</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B11">
-        <v>413.15701700490001</v>
-      </c>
-      <c r="C11">
-        <v>283.80408894206403</v>
-      </c>
-      <c r="D11">
-        <v>12.1201100575453</v>
+      <c r="B11" s="1">
+        <v>1104.74127909341</v>
+      </c>
+      <c r="C11" s="1">
+        <v>1083.3378819705299</v>
+      </c>
+      <c r="D11" s="1">
+        <v>25.968185889190199</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B12">
-        <v>405.486572735756</v>
-      </c>
-      <c r="C12">
-        <v>296.47528444909801</v>
-      </c>
-      <c r="D12">
-        <v>15.382458189411301</v>
+      <c r="B12" s="1">
+        <v>1107.01027655296</v>
+      </c>
+      <c r="C12" s="1">
+        <v>1167.08084741383</v>
+      </c>
+      <c r="D12" s="1">
+        <v>22.013294307367801</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B13">
-        <v>394.12374500052601</v>
-      </c>
-      <c r="C13">
-        <v>341.903520299543</v>
-      </c>
-      <c r="D13">
-        <v>11.4040332608049</v>
+      <c r="B13" s="1">
+        <v>1217.2519323551801</v>
+      </c>
+      <c r="C13" s="1">
+        <v>1173.3182906807899</v>
+      </c>
+      <c r="D13" s="1">
+        <v>23.566529125930501</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+      <c r="A14" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B14">
-        <v>475.72187534557702</v>
-      </c>
-      <c r="C14">
-        <v>338.38912602648799</v>
-      </c>
-      <c r="D14">
-        <v>12.5773850816046</v>
+      <c r="B14" s="1">
+        <v>1223.0172962603799</v>
+      </c>
+      <c r="C14" s="1">
+        <v>1219.6210184233701</v>
+      </c>
+      <c r="D14" s="1">
+        <v>27.633073682169599</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
+      <c r="A15" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B15">
-        <v>469.80660636387</v>
-      </c>
-      <c r="C15">
-        <v>367.64685364793098</v>
-      </c>
-      <c r="D15">
-        <v>15.783044946344599</v>
+      <c r="B15" s="1">
+        <v>1226.83194615723</v>
+      </c>
+      <c r="C15" s="1">
+        <v>1307.8043296753799</v>
+      </c>
+      <c r="D15" s="1">
+        <v>23.631188878050601</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
+      <c r="A16" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B16">
-        <v>461.62291510338201</v>
-      </c>
-      <c r="C16">
-        <v>430.140525115868</v>
-      </c>
-      <c r="D16">
-        <v>12.7830662957259</v>
+      <c r="B16" s="1">
+        <v>1341.37643230502</v>
+      </c>
+      <c r="C16" s="1">
+        <v>1316.02053701047</v>
+      </c>
+      <c r="D16" s="1">
+        <v>25.234793033555199</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
+      <c r="A17" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B17">
-        <v>543.86249777213197</v>
-      </c>
-      <c r="C17">
-        <v>420.86430426379297</v>
-      </c>
-      <c r="D17">
-        <v>13.985810380425299</v>
+      <c r="B17" s="1">
+        <v>1348.9014108670001</v>
+      </c>
+      <c r="C17" s="1">
+        <v>1365.32176378944</v>
+      </c>
+      <c r="D17" s="1">
+        <v>29.412304200546199</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
+      <c r="A18" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B18">
-        <v>541.79517373662804</v>
-      </c>
-      <c r="C18">
-        <v>446.99908309993998</v>
-      </c>
-      <c r="D18">
-        <v>17.251709240509999</v>
+      <c r="B18" s="1">
+        <v>1354.56668377764</v>
+      </c>
+      <c r="C18" s="1">
+        <v>1457.55400486645</v>
+      </c>
+      <c r="D18" s="1">
+        <v>25.305013447669499</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
+      <c r="A19" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B19">
-        <v>537.58610643166696</v>
-      </c>
-      <c r="C19">
-        <v>508.03033497733003</v>
-      </c>
-      <c r="D19">
-        <v>13.864351765265299</v>
+      <c r="B19" s="1">
+        <v>1473.38933933867</v>
+      </c>
+      <c r="C19" s="1">
+        <v>1468.1237195840499</v>
+      </c>
+      <c r="D19" s="1">
+        <v>26.959809087720402</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
+      <c r="A20" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B20">
-        <v>622.81455494182501</v>
-      </c>
-      <c r="C20">
-        <v>504.59226540652298</v>
-      </c>
-      <c r="D20">
-        <v>15.142865780454001</v>
+      <c r="B20" s="1">
+        <v>1482.6225875853099</v>
+      </c>
+      <c r="C20" s="1">
+        <v>1520.6803212592999</v>
+      </c>
+      <c r="D20" s="1">
+        <v>31.248826701506001</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
+      <c r="A21" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B21">
-        <v>619.40527903236705</v>
-      </c>
-      <c r="C21">
-        <v>532.52461009301896</v>
-      </c>
-      <c r="D21">
-        <v>18.626543809244701</v>
+      <c r="B21" s="1">
+        <v>1490.0481014501299</v>
+      </c>
+      <c r="C21" s="1">
+        <v>1617.19452644065</v>
+      </c>
+      <c r="D21" s="1">
+        <v>27.059111888675101</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
+      <c r="A22" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B22">
-        <v>613.34275839878501</v>
-      </c>
-      <c r="C22">
-        <v>596.04441104548403</v>
-      </c>
-      <c r="D22">
-        <v>14.985470209705801</v>
+      <c r="B22" s="1">
+        <v>1613.33522026162</v>
+      </c>
+      <c r="C22" s="1">
+        <v>1630.06488215073</v>
+      </c>
+      <c r="D22" s="1">
+        <v>28.7643355710977</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
+      <c r="A23" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B23">
-        <v>704.17503822338404</v>
-      </c>
-      <c r="C23">
-        <v>593.03881064761595</v>
-      </c>
-      <c r="D23">
-        <v>16.289173714830302</v>
+      <c r="B23" s="1">
+        <v>1624.37051038492</v>
+      </c>
+      <c r="C23" s="1">
+        <v>1686.0321217783401</v>
+      </c>
+      <c r="D23" s="1">
+        <v>33.160644854731601</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
+      <c r="A24" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B24">
-        <v>702.81513820482201</v>
-      </c>
-      <c r="C24">
-        <v>626.34405705040297</v>
-      </c>
-      <c r="D24">
-        <v>19.787801034550998</v>
+      <c r="B24" s="1">
+        <v>1633.67047630262</v>
+      </c>
+      <c r="C24" s="1">
+        <v>1786.99501883626</v>
+      </c>
+      <c r="D24" s="1">
+        <v>28.8921775523965</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
+      <c r="A25" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B25">
-        <v>699.30033527836099</v>
-      </c>
-      <c r="C25">
-        <v>696.33688561490806</v>
-      </c>
-      <c r="D25">
-        <v>16.345523921750001</v>
+      <c r="B25" s="1">
+        <v>1761.45019446775</v>
+      </c>
+      <c r="C25" s="1">
+        <v>1802.2880287979899</v>
+      </c>
+      <c r="D25" s="1">
+        <v>30.6494865299975</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
+      <c r="A26" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B26">
-        <v>792.93282276899504</v>
-      </c>
-      <c r="C26">
-        <v>694.283741761138</v>
-      </c>
-      <c r="D26">
-        <v>17.7054279303021</v>
+      <c r="B26" s="1">
+        <v>1774.39843087229</v>
+      </c>
+      <c r="C26" s="1">
+        <v>1861.6462905896899</v>
+      </c>
+      <c r="D26" s="1">
+        <v>35.158240454037497</v>
       </c>
     </row>
   </sheetData>

</xml_diff>